<commit_message>
refactor locations and documentation event
</commit_message>
<xml_diff>
--- a/events_template.xlsx
+++ b/events_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -28,24 +28,24 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
     <t xml:space="preserve">startDateTime</t>
   </si>
   <si>
     <t xml:space="preserve">endDateTime</t>
   </si>
   <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
     <t xml:space="preserve">Segundo evento actualizado</t>
   </si>
   <si>
     <t xml:space="preserve">Este es un evento genial</t>
   </si>
   <si>
-    <t xml:space="preserve">En Monteria</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024-03-23 01:29:29.593+00</t>
   </si>
   <si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Tercer evento actualizado</t>
   </si>
   <si>
-    <t xml:space="preserve">En Bucaramanga</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024-03-23 01:29:29.593+01</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cuarto evento actualizado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En Barranquilla</t>
   </si>
   <si>
     <t xml:space="preserve">2024-03-23 01:29:29.593+02</t>
@@ -182,20 +176,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.87"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -208,25 +203,31 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>4.695014</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>-74.116591</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -234,7 +235,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -242,25 +243,31 @@
       <c r="D3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>13</v>
+      <c r="E3" s="0" t="n">
+        <v>4.695014</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>-74.116591</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
+      <c r="E4" s="0" t="n">
+        <v>4.695014</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>-74.116591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>